<commit_message>
Automatische test-sync: 2025-07-27 16:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,8 +738,63 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-07-27 16:02:36</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -759,7 +814,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -767,17 +822,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -819,7 +874,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 16:23:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,8 +793,63 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-27 16:23:23</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -814,7 +869,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,17 +877,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -874,7 +929,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 17:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -848,8 +848,63 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-27 17:11:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -869,7 +924,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -877,17 +932,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -929,7 +984,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 17:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,8 +903,63 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-07-27 17:21:01</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -924,7 +979,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -932,17 +987,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -984,7 +1039,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 17:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -958,8 +958,63 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-07-27 17:54:51</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -979,7 +1034,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -987,17 +1042,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1039,7 +1094,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 18:18:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,15 +706,15 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Geachte klant,
-Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
+          <t>Geachte afzender,
+Dank u voor uw bericht. Om u beter van dienst te kunnen zijn, zou u meer details kunnen verstrekken over wat u precies wilt laten regelen? Hierdoor kunnen we u sneller en efficiënter helpen.
 Met vriendelijke groet,
 [Bedrijfsnaam] E-mailassistent</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-07-27 16:01:20</t>
+          <t>2025-07-27 18:18:39</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -735,286 +735,11 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>Nee</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Testmail #1: Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Overig</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Geachte klant,
-Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
-Met vriendelijke groet,
-[Bedrijfsnaam] E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-07-27 16:02:36</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Testmail #1: Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Overig</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Geachte klant,
-Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
-Met vriendelijke groet,
-[Bedrijfsnaam] E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-07-27 16:23:23</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Testmail #1: Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Overig</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Geachte klant,
-Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
-Met vriendelijke groet,
-[Bedrijfsnaam] E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-07-27 17:11:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Testmail #1: Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Overig</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Geachte klant,
-Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
-Met vriendelijke groet,
-[Bedrijfsnaam] E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-07-27 17:21:01</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Testmail #1: Kun jij dit even regelen?</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Overig</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Geachte klant,
-Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer informatie kunnen verstrekken over wat u precies wilt regelen?
-Met vriendelijke groet,
-[Bedrijfsnaam] E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-07-27 17:54:51</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Ja</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1034,7 +759,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1042,17 +767,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1094,7 +819,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 18:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -704,32 +704,24 @@
           <t>Overig</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Geachte afzender,
-Dank u voor uw bericht. Om u beter van dienst te kunnen zijn, zou u meer details kunnen verstrekken over wat u precies wilt laten regelen? Hierdoor kunnen we u sneller en efficiënter helpen.
-Met vriendelijke groet,
-[Bedrijfsnaam] E-mailassistent</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-07-27 18:18:39</t>
+          <t>2025-07-27 18:30:31</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Nee</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Ja</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 18:32:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,8 +730,64 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Zorg jij dat dit geregeld wordt?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #2: Zorg jij dat dit geregeld wordt?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om u beter te kunnen helpen, zou u meer specifieke informatie kunnen geven over welk aspect van onze service u graag geregeld zou willen hebben? Zo kunnen wij u adequaat assisteren. Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-07-27 18:32:43</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -751,7 +807,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -759,17 +815,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -811,7 +867,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 18:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,8 +786,64 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wil je dit voor me oppakken?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #3: Wil je dit voor me oppakken?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Kunt u meer details geven over wat precies moet worden opgepakt en welke specifieke actie er van ons wordt verwacht? Met meer informatie kan ik u beter van dienst zijn.
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-27 18:34:55</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -807,7 +863,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -815,17 +871,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -840,7 +896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,6 +926,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 18:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -842,8 +842,64 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun je dit intern bespreken?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #4: Kun je dit intern bespreken?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Kun je wat meer specifieke informatie geven over waarover je precies wilt dat er intern overlegd wordt? Op die manier kan ik ervoor zorgen dat je aanvraag bij de juiste persoon of afdeling terechtkomt.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-27 18:37:05</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -863,7 +919,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -871,17 +927,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -933,7 +989,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,202 +704,42 @@
           <t>Overig</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw bericht. Om u zo goed mogelijk van dienst te zijn, zou u wat meer details kunnen geven over wat u precies geregeld wilt hebben? Zo kunnen wij u beter helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-07-27 18:30:31</t>
+          <t>2025-07-27 19:11:15</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Nee</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Nee</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Zorg jij dat dit geregeld wordt?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Testmail #2: Zorg jij dat dit geregeld wordt?</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Overig</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Beste klant,
-Bedankt voor uw e-mail. Om u beter te kunnen helpen, zou u meer specifieke informatie kunnen geven over welk aspect van onze service u graag geregeld zou willen hebben? Zo kunnen wij u adequaat assisteren. Alvast bedankt voor uw medewerking.
-Met vriendelijke groet,
-[Naam]
-E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-07-27 18:32:43</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Wil je dit voor me oppakken?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Testmail #3: Wil je dit voor me oppakken?</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Beste klant,
-Bedankt voor uw bericht. Kunt u meer details geven over wat precies moet worden opgepakt en welke specifieke actie er van ons wordt verwacht? Met meer informatie kan ik u beter van dienst zijn.
-Met vriendelijke groet,
-[Naam] 
-E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-07-27 18:34:55</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Kun je dit intern bespreken?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>mailmind.test@zohomail.eu</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Testmail #4: Kun je dit intern bespreken?</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Beste afzender,
-Bedankt voor je e-mail. Kun je wat meer specifieke informatie geven over waarover je precies wilt dat er intern overlegd wordt? Op die manier kan ik ervoor zorgen dat je aanvraag bij de juiste persoon of afdeling terechtkomt.
-Met vriendelijke groet,
-[Naam]
-E-mailassistent</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-07-27 18:37:05</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Ja</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -919,7 +759,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -927,17 +767,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -952,7 +792,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,17 +819,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,8 +738,63 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw bericht. Om u zo goed mogelijk van dienst te zijn, zou u wat meer details kunnen geven over wat u precies geregeld wilt hebben? Zo kunnen wij u beter helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:12:17</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -759,7 +814,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -767,17 +822,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -819,7 +874,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:14:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,8 +793,64 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw e-mail. Om u zo goed mogelijk van dienst te kunnen zijn, wil ik u vragen om meer informatie te verstrekken over de specifieke kwestie die u wilt dat we oppakken. Kunt u mij wat meer details geven over wat u precies nodig heeft? Op die manier kunnen we u beter helpen.
+Met vriendelijke groet,
+[Naam van de e-mailassistent]
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:14:34</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -814,7 +870,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,17 +878,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -847,7 +903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -877,6 +933,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,8 +849,63 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw e-mail. Om uw vraag snel en adequaat te kunnen afhandelen, hebben we meer informatie van u nodig. Kunt u alstublieft specifiek aangeven wat uw vraag, probleem of verzoek is? Met deze informatie kunnen wij u zo goed mogelijk van dienst zijn.
+Met vriendelijke groet,
+[Bedrijfsnaam] e-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:16:48</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -870,7 +925,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -878,17 +933,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -930,7 +985,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -904,8 +904,63 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je interesse in het bestellen van M5-bouten. Helaas kan ik als e-mailassistent geen bestellingen plaatsen. Voor het bestellen van producten kun je terecht op onze website of contact opnemen met onze verkoopafdeling.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:18:59</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -925,7 +980,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -933,17 +988,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -958,7 +1013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -998,6 +1053,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -959,8 +959,64 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #5: Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Dank u voor uw bericht. Helaas kan ik niet achterhalen om welke klant het gaat op basis van de informatie die u heeft verstrekt. Kunt u mij de naam of het klantnummer van de desbetreffende klant geven, zodat ik dit verder kan onderzoeken?
+Met vriendelijke groet,
+[Naam van de e-mailassistent]
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:21:11</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -980,7 +1036,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -988,17 +1044,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1050,7 +1106,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:23:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1015,8 +1015,63 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Op dit moment hebben we nog voorraad van de EcoPro-700. U kunt deze bestellen via onze website of contact opnemen met onze verkoopafdeling voor meer informatie.
+Met vriendelijke groet,
+[Bedrijfsnaam] - Verkoopafdeling</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:23:23</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1036,7 +1091,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1044,17 +1099,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1069,7 +1124,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1119,6 +1174,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:25:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1070,8 +1070,60 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>FALLBACK_BLOCKED</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:25:33</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1091,7 +1143,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1099,17 +1151,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1167,17 +1219,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:27:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1122,8 +1122,55 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:27:45</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1143,7 +1190,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1151,17 +1198,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1209,17 +1256,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1169,8 +1169,64 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Beste,
+Dank voor je bericht. Om je zo goed mogelijk te kunnen helpen, zou je wat meer informatie met ons kunnen delen? Kun je aangeven waar je precies op wacht of waarover je meer wilt weten? Op die manier kunnen we je beter van dienst zijn.
+Met vriendelijke groet,  
+[Naam]  
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:29:55</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1190,7 +1246,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1198,17 +1254,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1250,7 +1306,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:32:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1225,8 +1225,64 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor uw e-mail. Helaas kan ik u op basis van de informatie uit uw e-mail niet vertellen waar u precies naar op zoek bent. Als u meer context kunt geven of details over het onderwerp kunt verstrekken, help ik u graag verder. 
+Met vriendelijke groet,
+[Je naam]
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:32:24</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1246,7 +1302,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1254,17 +1310,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1306,7 +1362,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1281,8 +1281,63 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mijn retour is nog steeds niet verwerkt.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u wel voor uw e-mail. Om u beter van dienst te kunnen zijn, ontvangen wij graag wat meer informatie om uw retourzending te kunnen traceren. Kunt u ons uw ordernummer en de datum van retournering verstrekken? Op die manier kunnen we uw zaak nauwkeurig onderzoeken en u van dienst zijn.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:34:37</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1302,7 +1357,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1310,17 +1365,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1335,7 +1390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1395,6 +1450,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1336,8 +1336,63 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #12: Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw bericht. Als u nog geen geld terug heeft ontvangen, zou dat kunnen betekenen dat de terugbetaling nog niet is verwerkt. Zou u ons uw transactiegegevens en/of bestelnummer kunnen doorgeven, zodat we dit verder kunnen onderzoeken en u van dienst kunnen zijn?
+Met vriendelijke groet,
+[Naam van het bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:36:55</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1357,7 +1412,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1365,17 +1420,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1443,17 +1498,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1391,8 +1391,65 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Beste heer/mevrouw,
+Bedankt voor uw interesse in de VentiQ-250. Helaas kan ik u op dit moment geen datasheet van de VentiQ-250 sturen, omdat ik geen e-mailbijlage kan openen.
+U kunt de datasheet van de VentiQ-250 vinden op onze website [www.bedrijfsnaam.nl] onder het tabblad 'Producten'. Mocht u nog verdere vragen hebben, dan help ik u graag verder.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:39:08</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1412,7 +1469,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1420,17 +1477,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1482,7 +1539,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1448,8 +1448,64 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Beste sender,
+Bedankt voor je e-mail. Om je vraag over de CE-certificaten van het product te beantwoorden, heb ik wat meer informatie nodig. Kun je het productnummer of de naam van het product doorgeven, zodat ik de relevante certificaten kan opzoeken? 
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:41:20</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1469,7 +1525,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1477,17 +1533,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1539,7 +1595,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1504,8 +1504,63 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Kunt u meer specifieke informatie geven over wat u graag met Koen zou willen bespreken? Zo kunnen we ervoor zorgen dat uw boodschap zo effectief mogelijk wordt doorgegeven.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:43:35</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1525,7 +1580,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1533,17 +1588,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1605,7 +1660,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1559,8 +1559,63 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Kun je me iets meer informatie geven over welk specifiek document of welke informatie je wilt laten doorsturen? Dan kan ik je beter helpen.
+Met vriendelijke groet,
+[Naam Bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:45:48</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1580,7 +1635,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1588,17 +1643,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1660,7 +1715,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1614,8 +1614,63 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je e-mail. Wij zullen proberen om de demo in te plannen bij Van Dijk op vrijdag om 11:00 uur. 
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:48:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1635,7 +1690,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1643,17 +1698,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1668,7 +1723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1738,6 +1793,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:50:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1669,8 +1669,63 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Geachte afzender,
+Bedankt voor uw e-mail. Het lijkt erop dat deze e-mail bedoeld is als een testmail. Als u daadwerkelijk 200 stuks M8-bouten RVS wenst te bestellen voor Van Dijk, kunt u ons uw bestelgegevens sturen naar het juiste e-mailadres voor bestellingen. Mocht u verdere assistentie nodig hebben of vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:50:12</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1690,7 +1745,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1698,17 +1753,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1776,7 +1831,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1786,11 +1841,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1724,8 +1724,63 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #19: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Beste [naam],
+Dank voor je e-mail. Om je verzoek efficiënt te kunnen verwerken, zouden we graag wat meer informatie ontvangen. Zou je zo vriendelijk willen zijn om de contactgegevens van klant Jansen met ons te delen, zodat we contact met hem kunnen opnemen?
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:52:27</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1745,7 +1800,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1753,17 +1808,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1811,7 +1866,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1821,11 +1876,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-27 19:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-27.xlsx
+++ b/logs/mail_log_2025-07-27.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1779,8 +1779,63 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #20: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw e-mail. Ik begrijp dat u niet tevreden bent over het proces. Om uw zorgen beter te kunnen begrijpen en aanpakken, zou u meer specifieke details kunnen delen over wat er precies is misgegaan?
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-07-27 19:54:38</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1800,7 +1855,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1808,17 +1863,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1833,7 +1888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1913,6 +1968,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>